<commit_message>
FEAT: Importation du MCD-MLD-MPD.
</commit_message>
<xml_diff>
--- a/Dictionnaire_données_Films.xlsx
+++ b/Dictionnaire_données_Films.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherb\Desktop\scolaire amel\M2 MIASHS 2024_2025\Architecture Web\TP_Not-_Archi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696ADF39-BE47-4C44-A67E-E4416E72D29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E143173-14FA-4C1F-A5A2-27ADD3D0CF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -141,9 +141,6 @@
     <t>Identifiant de l'acteur</t>
   </si>
   <si>
-    <t>role_favoris</t>
-  </si>
-  <si>
     <t>Rôle préféré de l'utilisateur.</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t xml:space="preserve">Identifiant de l'utilisateur. </t>
+  </si>
+  <si>
+    <t>role_favori</t>
   </si>
 </sst>
 </file>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,13 +638,13 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -693,13 +693,13 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>